<commit_message>
Risultati 16 e 79 suplin e quad
</commit_message>
<xml_diff>
--- a/F16_truncated/results_f16_suplin.xlsx
+++ b/F16_truncated/results_f16_suplin.xlsx
@@ -16,6 +16,9 @@
     <sheet name="niter_5" sheetId="9" r:id="rId11"/>
     <sheet name="f_val_5" sheetId="10" r:id="rId12"/>
     <sheet name="ExactComparison" sheetId="11" r:id="rId13"/>
+    <sheet name="bt_3" sheetId="12" r:id="rId14"/>
+    <sheet name="cg_3" sheetId="13" r:id="rId15"/>
+    <sheet name="n_conv3" sheetId="14" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t>Row</t>
   </si>
@@ -314,6 +317,186 @@
   </si>
   <si>
     <t>n=10^5</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
   </si>
 </sst>
 </file>
@@ -334,7 +517,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -352,11 +535,17 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -368,6 +557,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,6 +738,297 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="12.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
+    <col min="4" max="4" width="12.7109375" customWidth="true"/>
+    <col min="5" max="5" width="12.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="8" max="8" width="12.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.50157308070351558</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.43146324689802951</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.36852160520638788</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.46114859375728934</v>
+      </c>
+      <c r="F2" s="0">
+        <v>0.46114859375728934</v>
+      </c>
+      <c r="G2" s="0">
+        <v>0.46114859375728934</v>
+      </c>
+      <c r="H2" s="0">
+        <v>0.46114859375728934</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0.42518552875695736</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.41514874014874015</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.41624585559368177</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0.45023559773559774</v>
+      </c>
+      <c r="F3" s="0">
+        <v>0.46114859375728934</v>
+      </c>
+      <c r="G3" s="0">
+        <v>0.46114859375728934</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0.46114859375728934</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="11.7109375" customWidth="true"/>
+    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="11.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="0">
+        <v>13.21628845389715</v>
+      </c>
+      <c r="C2" s="0">
+        <v>13.134415186263013</v>
+      </c>
+      <c r="D2" s="0">
+        <v>13.245764018590107</v>
+      </c>
+      <c r="E2" s="0">
+        <v>13.56649996541301</v>
+      </c>
+      <c r="F2" s="0">
+        <v>13.56649996541301</v>
+      </c>
+      <c r="G2" s="0">
+        <v>13.56649996541301</v>
+      </c>
+      <c r="H2" s="0">
+        <v>13.56649996541301</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="0">
+        <v>13.02899196042053</v>
+      </c>
+      <c r="C3" s="0">
+        <v>12.853978428978429</v>
+      </c>
+      <c r="D3" s="0">
+        <v>13.220391094412836</v>
+      </c>
+      <c r="E3" s="0">
+        <v>13.479692807192809</v>
+      </c>
+      <c r="F3" s="0">
+        <v>13.56649996541301</v>
+      </c>
+      <c r="G3" s="0">
+        <v>13.56649996541301</v>
+      </c>
+      <c r="H3" s="0">
+        <v>13.56649996541301</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="6.82421875" customWidth="true"/>
+    <col min="3" max="3" width="6.82421875" customWidth="true"/>
+    <col min="4" max="4" width="6.82421875" customWidth="true"/>
+    <col min="5" max="5" width="6.82421875" customWidth="true"/>
+    <col min="6" max="6" width="7.82421875" customWidth="true"/>
+    <col min="7" max="7" width="7.82421875" customWidth="true"/>
+    <col min="8" max="8" width="5.6015625" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="0">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0">
+        <v>9</v>
+      </c>
+      <c r="G2" s="0">
+        <v>9</v>
+      </c>
+      <c r="H2" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0">
+        <v>9</v>
+      </c>
+      <c r="G3" s="0">
+        <v>9</v>
+      </c>
+      <c r="H3" s="0">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
@@ -550,8 +1036,8 @@
   <cols>
     <col min="1" max="1" width="4.82421875" customWidth="true"/>
     <col min="2" max="2" width="10.7109375" customWidth="true"/>
-    <col min="3" max="3" width="9.7109375" customWidth="true"/>
-    <col min="4" max="4" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="10.7109375" customWidth="true"/>
+    <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="14.7109375" customWidth="true"/>
     <col min="6" max="6" width="14.7109375" customWidth="true"/>
     <col min="7" max="7" width="14.7109375" customWidth="true"/>
@@ -560,80 +1046,80 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="B2" s="0">
-        <v>0.0064322900000000002</v>
+        <v>0.0095995099999999986</v>
       </c>
       <c r="C2" s="0">
-        <v>0.0067285000000000001</v>
+        <v>0.0092480800000000005</v>
       </c>
       <c r="D2" s="0">
-        <v>0.0066879000000000001</v>
+        <v>0.0095053875000000003</v>
       </c>
       <c r="E2" s="0">
-        <v>0.0061348333333333333</v>
+        <v>0.0090722555555555542</v>
       </c>
       <c r="F2" s="0">
-        <v>0.0064202777777777782</v>
+        <v>0.0089183444444444447</v>
       </c>
       <c r="G2" s="0">
-        <v>0.0062301555555555558</v>
+        <v>0.0094174333333333343</v>
       </c>
       <c r="H2" s="0">
-        <v>0.010122822222222223</v>
+        <v>0.021389933333333336</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B3" s="0">
-        <v>0.034042200000000002</v>
+        <v>0.044539528571428566</v>
       </c>
       <c r="C3" s="0">
-        <v>0.031639911111111113</v>
+        <v>0.043413455555555557</v>
       </c>
       <c r="D3" s="0">
-        <v>0.031975700000000003</v>
+        <v>0.044360990000000003</v>
       </c>
       <c r="E3" s="0">
-        <v>0.031879499999999998</v>
+        <v>0.044145809999999994</v>
       </c>
       <c r="F3" s="0">
-        <v>0.032323744444444441</v>
+        <v>0.043229844444444457</v>
       </c>
       <c r="G3" s="0">
-        <v>0.032189477777777781</v>
+        <v>0.042292066666666663</v>
       </c>
       <c r="H3" s="0">
-        <v>0.010122822222222223</v>
+        <v>0.021389933333333336</v>
       </c>
     </row>
   </sheetData>
@@ -657,33 +1143,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="B2" s="0">
         <v>22.5</v>
@@ -709,7 +1195,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="B3" s="0">
         <v>22.428571428571427</v>
@@ -754,33 +1240,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>28</v>
+        <v>125</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="B2" s="0">
         <v>-427.40447637484948</v>
@@ -806,7 +1292,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="B3" s="0">
         <v>-427.40447637484931</v>

</xml_diff>